<commit_message>
Updated Messages and added a port for deployment purpose
</commit_message>
<xml_diff>
--- a/src/data/quiz.xlsx
+++ b/src/data/quiz.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">explanation</t>
   </si>
   <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imageUrl</t>
+  </si>
+  <si>
     <t xml:space="preserve">All of the following highly specialised cells are dependent solely on aerobic respiration for ATP generation and thus these tissues suffer from ill-effects of ischaemia more severely and rapidly except</t>
   </si>
   <si>
@@ -131,6 +137,15 @@
   </si>
   <si>
     <t xml:space="preserve">Immunity is a ‘double-edged sword’—it protects the host against various injurious agents but may also turn lethal and cause cell injury, such as hypersensitivity reactions, anaphylactic reactions, and autoimmune diseases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypoxia, Chemicals or drugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://imgs.search.brave.com/_qmLdsZ_CvoIFVn153ro9Lf9Gh_LGtHQKnvg2rZpAC0/rs:fit:500:0:0:0/g:ce/aHR0cHM6Ly9pbWFn/ZXMuZ2VuaWFsbHku/Y29tL2dlbmlhbC5s/eS9nZW5pYWxseS90/ZW1wbGF0ZXMvNTEw/OTNlNWUtZDYyOC00/NWQxLTk5MzgtOGJh/NzM3NGRiODk0Lmpw/ZWc</t>
   </si>
 </sst>
 </file>
@@ -140,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +185,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,13 +242,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -422,10 +459,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -452,330 +489,368 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="F16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>36</v>
+      <c r="H16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I16" r:id="rId1" display="https://imgs.search.brave.com/_qmLdsZ_CvoIFVn153ro9Lf9Gh_LGtHQKnvg2rZpAC0/rs:fit:500:0:0:0/g:ce/aHR0cHM6Ly9pbWFn/ZXMuZ2VuaWFsbHku/Y29tL2dlbmlhbC5s/eS9nZW5pYWxseS90/ZW1wbGF0ZXMvNTEw/OTNlNWUtZDYyOC00/NWQxLTk5MzgtOGJh/NzM3NGRiODk0Lmpw/ZWc"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>